<commit_message>
6MWT updated to include categories, no implementation option at the moment
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_QRS_6MWT.xlsx
+++ b/curation/draft/collection/collection_specialization_QRS_6MWT.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DA25EC-0D12-4279-8ADF-D8AD59F6328D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7663B35A-7D5C-364C-94E3-C1D9B6918987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_QRS_6MWT" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_QRS_6MWT!$A$1:$AG$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_QRS_6MWT!$A$1:$AH$17</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="130">
   <si>
     <t>package_date</t>
   </si>
@@ -410,6 +410,9 @@
   </si>
   <si>
     <t>SIXMW1_FTASTDEV</t>
+  </si>
+  <si>
+    <t>categories</t>
   </si>
 </sst>
 </file>
@@ -788,50 +791,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG17"/>
+  <dimension ref="A1:AH17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="35.140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="28.140625" style="2" customWidth="1"/>
-    <col min="31" max="31" width="58.7109375" style="2" customWidth="1"/>
-    <col min="32" max="32" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.85546875" style="2"/>
+    <col min="11" max="11" width="13" style="2" customWidth="1"/>
+    <col min="12" max="12" width="30.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.6640625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="35.1640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="28.1640625" style="2" customWidth="1"/>
+    <col min="32" max="32" width="58.6640625" style="2" customWidth="1"/>
+    <col min="33" max="33" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -863,76 +867,79 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
@@ -949,56 +956,56 @@
       <c r="H2" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
         <v>1</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>1</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>42</v>
       </c>
@@ -1015,41 +1022,41 @@
       <c r="H3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>2</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>10</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="AE3" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="AF3" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>42</v>
       </c>
@@ -1066,50 +1073,50 @@
       <c r="H4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>3</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T4" s="2">
+      <c r="U4" s="2">
         <v>50</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="Y4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="2" t="s">
+      <c r="AC4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="AD4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AE4" s="2" t="s">
+      <c r="AF4" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1126,41 +1133,41 @@
       <c r="H5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <v>4</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T5" s="2">
+      <c r="U5" s="2">
         <v>200</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AE5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AE5" s="2" t="s">
+      <c r="AF5" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>60</v>
       </c>
@@ -1179,41 +1186,41 @@
       <c r="H6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="R6" s="2">
         <v>1</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="T6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T6" s="2">
+      <c r="U6" s="2">
         <v>3</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AE6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AE6" s="2" t="s">
+      <c r="AF6" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>60</v>
       </c>
@@ -1232,53 +1239,53 @@
       <c r="H7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="R7" s="2">
         <v>2</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="T7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T7" s="2">
+      <c r="U7" s="2">
         <v>1</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="X7" s="2" t="s">
+      <c r="Y7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB7" s="2" t="s">
+      <c r="AC7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC7" s="2" t="s">
+      <c r="AD7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AD7" s="2" t="s">
+      <c r="AE7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AE7" s="2" t="s">
+      <c r="AF7" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>78</v>
       </c>
@@ -1297,41 +1304,41 @@
       <c r="H8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="R8" s="2">
         <v>1</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="T8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T8" s="2">
+      <c r="U8" s="2">
         <v>3</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AE8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AF8" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>78</v>
       </c>
@@ -1350,53 +1357,53 @@
       <c r="H9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="Q9" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="R9" s="2">
         <v>2</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="S9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="T9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T9" s="2">
+      <c r="U9" s="2">
         <v>1</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="X9" s="2" t="s">
+      <c r="Y9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB9" s="2" t="s">
+      <c r="AC9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC9" s="2" t="s">
+      <c r="AD9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AD9" s="2" t="s">
+      <c r="AE9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AE9" s="2" t="s">
+      <c r="AF9" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>85</v>
       </c>
@@ -1415,41 +1422,41 @@
       <c r="H10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="Q10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="R10" s="2">
         <v>1</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S10" s="2" t="s">
+      <c r="T10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T10" s="2">
+      <c r="U10" s="2">
         <v>3</v>
       </c>
-      <c r="AD10" s="2" t="s">
+      <c r="AE10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AE10" s="2" t="s">
+      <c r="AF10" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>85</v>
       </c>
@@ -1468,53 +1475,53 @@
       <c r="H11" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="R11" s="2">
         <v>2</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="S11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S11" s="2" t="s">
+      <c r="T11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T11" s="2">
+      <c r="U11" s="2">
         <v>1</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="X11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="X11" s="2" t="s">
+      <c r="Y11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB11" s="2" t="s">
+      <c r="AC11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC11" s="2" t="s">
+      <c r="AD11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AE11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AE11" s="2" t="s">
+      <c r="AF11" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>92</v>
       </c>
@@ -1533,41 +1540,41 @@
       <c r="H12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="Q12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="R12" s="2">
         <v>1</v>
       </c>
-      <c r="R12" s="2" t="s">
+      <c r="S12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="T12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T12" s="2">
+      <c r="U12" s="2">
         <v>3</v>
       </c>
-      <c r="AD12" s="2" t="s">
+      <c r="AE12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AE12" s="2" t="s">
+      <c r="AF12" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>92</v>
       </c>
@@ -1586,53 +1593,53 @@
       <c r="H13" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="Q13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="R13" s="2">
         <v>2</v>
       </c>
-      <c r="R13" s="2" t="s">
+      <c r="S13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="T13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T13" s="2">
+      <c r="U13" s="2">
         <v>1</v>
       </c>
-      <c r="W13" s="2" t="s">
+      <c r="X13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="X13" s="2" t="s">
+      <c r="Y13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB13" s="2" t="s">
+      <c r="AC13" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC13" s="2" t="s">
+      <c r="AD13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AD13" s="2" t="s">
+      <c r="AE13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AE13" s="2" t="s">
+      <c r="AF13" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>99</v>
       </c>
@@ -1651,41 +1658,41 @@
       <c r="H14" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="Q14" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="R14" s="2">
         <v>1</v>
       </c>
-      <c r="R14" s="2" t="s">
+      <c r="S14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S14" s="2" t="s">
+      <c r="T14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T14" s="2">
+      <c r="U14" s="2">
         <v>3</v>
       </c>
-      <c r="AD14" s="2" t="s">
+      <c r="AE14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AE14" s="2" t="s">
+      <c r="AF14" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>99</v>
       </c>
@@ -1704,53 +1711,53 @@
       <c r="H15" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="Q15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="R15" s="2">
         <v>2</v>
       </c>
-      <c r="R15" s="2" t="s">
+      <c r="S15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S15" s="2" t="s">
+      <c r="T15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T15" s="2">
+      <c r="U15" s="2">
         <v>1</v>
       </c>
-      <c r="W15" s="2" t="s">
+      <c r="X15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="X15" s="2" t="s">
+      <c r="Y15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB15" s="2" t="s">
+      <c r="AC15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC15" s="2" t="s">
+      <c r="AD15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AD15" s="2" t="s">
+      <c r="AE15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AE15" s="2" t="s">
+      <c r="AF15" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>106</v>
       </c>
@@ -1769,41 +1776,41 @@
       <c r="H16" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="Q16" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="R16" s="2">
         <v>1</v>
       </c>
-      <c r="R16" s="2" t="s">
+      <c r="S16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S16" s="2" t="s">
+      <c r="T16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T16" s="2">
+      <c r="U16" s="2">
         <v>3</v>
       </c>
-      <c r="AD16" s="2" t="s">
+      <c r="AE16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AE16" s="2" t="s">
+      <c r="AF16" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>106</v>
       </c>
@@ -1822,54 +1829,54 @@
       <c r="H17" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="Q17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="R17" s="2">
         <v>2</v>
       </c>
-      <c r="R17" s="2" t="s">
+      <c r="S17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S17" s="2" t="s">
+      <c r="T17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T17" s="2">
+      <c r="U17" s="2">
         <v>1</v>
       </c>
-      <c r="W17" s="2" t="s">
+      <c r="X17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="X17" s="2" t="s">
+      <c r="Y17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB17" s="2" t="s">
+      <c r="AC17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC17" s="2" t="s">
+      <c r="AD17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AD17" s="2" t="s">
+      <c r="AE17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AE17" s="2" t="s">
+      <c r="AF17" s="2" t="s">
         <v>124</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AH17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
QRS changed for annotation of the --STAT item to remove the condition ..when --TESTCD = --ALL: this is not applicable for QRS instruments per feedback from eCRF portal team
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_QRS_6MWT.xlsx
+++ b/curation/draft/collection/collection_specialization_QRS_6MWT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7663B35A-7D5C-364C-94E3-C1D9B6918987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF508311-FD6E-AF49-828C-989129208365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,9 +178,6 @@
     <t>Single</t>
   </si>
   <si>
-    <t>[NOT SUBMITTED]; FTSTAT = NOT DONE when FTTESTCD = FTALL</t>
-  </si>
-  <si>
     <t>FTDAT</t>
   </si>
   <si>
@@ -413,6 +410,9 @@
   </si>
   <si>
     <t>categories</t>
+  </si>
+  <si>
+    <t>[NOT SUBMITTED]; FTSTAT = NOT DONE</t>
   </si>
 </sst>
 </file>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF17" sqref="AF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -867,7 +867,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
@@ -954,19 +954,19 @@
         <v>35</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="M2" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>44</v>
@@ -999,10 +999,10 @@
         <v>50</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -1020,22 +1020,22 @@
         <v>35</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="M3" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="R3" s="2">
         <v>2</v>
@@ -1044,16 +1044,16 @@
         <v>38</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U3" s="2">
         <v>10</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="16" x14ac:dyDescent="0.2">
@@ -1071,13 +1071,13 @@
         <v>35</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="M4" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>36</v>
@@ -1113,7 +1113,7 @@
         <v>36</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="16" x14ac:dyDescent="0.2">
@@ -1131,22 +1131,22 @@
         <v>35</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="M5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="R5" s="2">
         <v>4</v>
@@ -1161,18 +1161,18 @@
         <v>200</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>33</v>
@@ -1184,22 +1184,22 @@
         <v>35</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="R6" s="2">
         <v>1</v>
@@ -1208,24 +1208,24 @@
         <v>38</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U6" s="2">
         <v>3</v>
       </c>
       <c r="AE6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF6" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="AF6" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>33</v>
@@ -1237,22 +1237,22 @@
         <v>35</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="M7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="R7" s="2">
         <v>2</v>
@@ -1267,30 +1267,30 @@
         <v>1</v>
       </c>
       <c r="X7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Y7" s="2" t="s">
+      <c r="AC7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AC7" s="2" t="s">
+      <c r="AD7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AD7" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AE7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>33</v>
@@ -1302,22 +1302,22 @@
         <v>35</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="R8" s="2">
         <v>1</v>
@@ -1326,24 +1326,24 @@
         <v>38</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U8" s="2">
         <v>3</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>33</v>
@@ -1355,22 +1355,22 @@
         <v>35</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="M9" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="Q9" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="R9" s="2">
         <v>2</v>
@@ -1385,30 +1385,30 @@
         <v>1</v>
       </c>
       <c r="X9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Y9" s="2" t="s">
+      <c r="AC9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AC9" s="2" t="s">
+      <c r="AD9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AD9" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AE9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>33</v>
@@ -1420,22 +1420,22 @@
         <v>35</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q10" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="R10" s="2">
         <v>1</v>
@@ -1444,24 +1444,24 @@
         <v>38</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U10" s="2">
         <v>3</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>33</v>
@@ -1473,22 +1473,22 @@
         <v>35</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="M11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="R11" s="2">
         <v>2</v>
@@ -1503,30 +1503,30 @@
         <v>1</v>
       </c>
       <c r="X11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Y11" s="2" t="s">
+      <c r="AC11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AC11" s="2" t="s">
+      <c r="AD11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AD11" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AE11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF11" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>33</v>
@@ -1538,22 +1538,22 @@
         <v>35</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="R12" s="2">
         <v>1</v>
@@ -1562,24 +1562,24 @@
         <v>38</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U12" s="2">
         <v>3</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>33</v>
@@ -1591,22 +1591,22 @@
         <v>35</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="M13" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="Q13" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="R13" s="2">
         <v>2</v>
@@ -1621,30 +1621,30 @@
         <v>1</v>
       </c>
       <c r="X13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Y13" s="2" t="s">
+      <c r="AC13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AC13" s="2" t="s">
+      <c r="AD13" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AD13" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AE13" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF13" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>33</v>
@@ -1656,22 +1656,22 @@
         <v>35</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="N14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q14" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="R14" s="2">
         <v>1</v>
@@ -1680,24 +1680,24 @@
         <v>38</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U14" s="2">
         <v>3</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>33</v>
@@ -1709,22 +1709,22 @@
         <v>35</v>
       </c>
       <c r="H15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="M15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="Q15" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="R15" s="2">
         <v>2</v>
@@ -1739,30 +1739,30 @@
         <v>1</v>
       </c>
       <c r="X15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Y15" s="2" t="s">
+      <c r="AC15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AC15" s="2" t="s">
+      <c r="AD15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AD15" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AE15" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF15" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>33</v>
@@ -1774,22 +1774,22 @@
         <v>35</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="R16" s="2">
         <v>1</v>
@@ -1798,24 +1798,24 @@
         <v>38</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U16" s="2">
         <v>3</v>
       </c>
       <c r="AE16" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF16" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="2:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>33</v>
@@ -1827,22 +1827,22 @@
         <v>35</v>
       </c>
       <c r="H17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="M17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="Q17" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="R17" s="2">
         <v>2</v>
@@ -1857,22 +1857,22 @@
         <v>1</v>
       </c>
       <c r="X17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Y17" s="2" t="s">
+      <c r="AC17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AC17" s="2" t="s">
+      <c r="AD17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AD17" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AE17" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF17" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added derivation columns (blank) - QRS_6MWT
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_QRS_6MWT.xlsx
+++ b/curation/draft/collection/collection_specialization_QRS_6MWT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF508311-FD6E-AF49-828C-989129208365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17ED749D-2F9E-9C40-8D57-3E3F23299E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Collection_QRS_6MWT" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_QRS_6MWT!$A$1:$AH$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_QRS_6MWT!$A$1:$AJ$17</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="132">
   <si>
     <t>package_date</t>
   </si>
@@ -413,6 +413,12 @@
   </si>
   <si>
     <t>[NOT SUBMITTED]; FTSTAT = NOT DONE</t>
+  </si>
+  <si>
+    <t>derived_variable</t>
+  </si>
+  <si>
+    <t>derivation_description</t>
   </si>
 </sst>
 </file>
@@ -791,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH17"/>
+  <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF17" sqref="AF17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -822,20 +828,21 @@
     <col min="21" max="21" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="28.1640625" style="2" customWidth="1"/>
-    <col min="32" max="32" width="58.6640625" style="2" customWidth="1"/>
-    <col min="33" max="33" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="8.83203125" style="2"/>
+    <col min="24" max="25" width="19.33203125" style="2" customWidth="1"/>
+    <col min="26" max="26" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28.1640625" style="2" customWidth="1"/>
+    <col min="34" max="34" width="58.6640625" style="2" customWidth="1"/>
+    <col min="35" max="35" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -906,40 +913,46 @@
         <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
@@ -983,29 +996,29 @@
       <c r="U2" s="2">
         <v>1</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>42</v>
       </c>
@@ -1049,14 +1062,14 @@
       <c r="U3" s="2">
         <v>10</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>42</v>
       </c>
@@ -1097,26 +1110,26 @@
       <c r="U4" s="2">
         <v>50</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="AA4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AF4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AE4" s="2" t="s">
+      <c r="AG4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AH4" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1160,14 +1173,14 @@
       <c r="U5" s="2">
         <v>200</v>
       </c>
-      <c r="AE5" s="2" t="s">
+      <c r="AG5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AF5" s="2" t="s">
+      <c r="AH5" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>59</v>
       </c>
@@ -1213,14 +1226,14 @@
       <c r="U6" s="2">
         <v>3</v>
       </c>
-      <c r="AE6" s="2" t="s">
+      <c r="AG6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AH6" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>59</v>
       </c>
@@ -1266,26 +1279,26 @@
       <c r="U7" s="2">
         <v>1</v>
       </c>
-      <c r="X7" s="2" t="s">
+      <c r="Z7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Y7" s="2" t="s">
+      <c r="AA7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AC7" s="2" t="s">
+      <c r="AE7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AD7" s="2" t="s">
+      <c r="AF7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AE7" s="2" t="s">
+      <c r="AG7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AF7" s="2" t="s">
+      <c r="AH7" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>77</v>
       </c>
@@ -1331,14 +1344,14 @@
       <c r="U8" s="2">
         <v>3</v>
       </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AG8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AF8" s="2" t="s">
+      <c r="AH8" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>77</v>
       </c>
@@ -1384,26 +1397,26 @@
       <c r="U9" s="2">
         <v>1</v>
       </c>
-      <c r="X9" s="2" t="s">
+      <c r="Z9" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Y9" s="2" t="s">
+      <c r="AA9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AC9" s="2" t="s">
+      <c r="AE9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AD9" s="2" t="s">
+      <c r="AF9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AE9" s="2" t="s">
+      <c r="AG9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AF9" s="2" t="s">
+      <c r="AH9" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>84</v>
       </c>
@@ -1449,14 +1462,14 @@
       <c r="U10" s="2">
         <v>3</v>
       </c>
-      <c r="AE10" s="2" t="s">
+      <c r="AG10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AF10" s="2" t="s">
+      <c r="AH10" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>84</v>
       </c>
@@ -1502,26 +1515,26 @@
       <c r="U11" s="2">
         <v>1</v>
       </c>
-      <c r="X11" s="2" t="s">
+      <c r="Z11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Y11" s="2" t="s">
+      <c r="AA11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AC11" s="2" t="s">
+      <c r="AE11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AF11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AE11" s="2" t="s">
+      <c r="AG11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AF11" s="2" t="s">
+      <c r="AH11" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>91</v>
       </c>
@@ -1567,14 +1580,14 @@
       <c r="U12" s="2">
         <v>3</v>
       </c>
-      <c r="AE12" s="2" t="s">
+      <c r="AG12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AF12" s="2" t="s">
+      <c r="AH12" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>91</v>
       </c>
@@ -1620,26 +1633,26 @@
       <c r="U13" s="2">
         <v>1</v>
       </c>
-      <c r="X13" s="2" t="s">
+      <c r="Z13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Y13" s="2" t="s">
+      <c r="AA13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AC13" s="2" t="s">
+      <c r="AE13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AD13" s="2" t="s">
+      <c r="AF13" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AE13" s="2" t="s">
+      <c r="AG13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AF13" s="2" t="s">
+      <c r="AH13" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>98</v>
       </c>
@@ -1685,14 +1698,14 @@
       <c r="U14" s="2">
         <v>3</v>
       </c>
-      <c r="AE14" s="2" t="s">
+      <c r="AG14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AF14" s="2" t="s">
+      <c r="AH14" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>98</v>
       </c>
@@ -1738,26 +1751,26 @@
       <c r="U15" s="2">
         <v>1</v>
       </c>
-      <c r="X15" s="2" t="s">
+      <c r="Z15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Y15" s="2" t="s">
+      <c r="AA15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AC15" s="2" t="s">
+      <c r="AE15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AD15" s="2" t="s">
+      <c r="AF15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AE15" s="2" t="s">
+      <c r="AG15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AF15" s="2" t="s">
+      <c r="AH15" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>105</v>
       </c>
@@ -1803,14 +1816,14 @@
       <c r="U16" s="2">
         <v>3</v>
       </c>
-      <c r="AE16" s="2" t="s">
+      <c r="AG16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AF16" s="2" t="s">
+      <c r="AH16" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="2:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>105</v>
       </c>
@@ -1856,27 +1869,27 @@
       <c r="U17" s="2">
         <v>1</v>
       </c>
-      <c r="X17" s="2" t="s">
+      <c r="Z17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Y17" s="2" t="s">
+      <c r="AA17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AC17" s="2" t="s">
+      <c r="AE17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AD17" s="2" t="s">
+      <c r="AF17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AE17" s="2" t="s">
+      <c r="AG17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AF17" s="2" t="s">
+      <c r="AH17" s="2" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AJ17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>